<commit_message>
updated experiment to split timelogs by experiment
</commit_message>
<xml_diff>
--- a/notes_II/checklist.xlsx
+++ b/notes_II/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte/Documents/global_scripts/pypetting_experiments/CombinationExperiment/notes_II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDDEE07-7C85-9744-A26E-CDAE7092E0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C084E7-44EB-9143-AE63-27A28B3B1F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="1200" windowWidth="35840" windowHeight="21900" xr2:uid="{650E8647-512E-6F4B-9ECD-036497EF412F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{650E8647-512E-6F4B-9ECD-036497EF412F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>LB in Trough</t>
   </si>
@@ -71,20 +71,23 @@
     <t>Prep Pintool &amp;  Reservoirs</t>
   </si>
   <si>
-    <t>Compile Worklist with comb-idx</t>
-  </si>
-  <si>
     <t>PD-Curve Checklist</t>
   </si>
   <si>
     <t>Tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IIb (and not for IIa) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Add second 12 Col overnight with prefilled columns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,6 +100,20 @@
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,14 +146,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +506,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +516,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -510,7 +542,7 @@
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -652,19 +684,23 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
earlier distribution to helper to reduce within exp inoculum variance. also changed next-day helper to be infected by the to-day assay
</commit_message>
<xml_diff>
--- a/notes_II/checklist.xlsx
+++ b/notes_II/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte/Documents/global_scripts/pypetting_experiments/CombinationExperiment/notes_II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C084E7-44EB-9143-AE63-27A28B3B1F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC25D4D-B0FF-9344-A383-AE3390775308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{650E8647-512E-6F4B-9ECD-036497EF412F}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>LB in Trough</t>
   </si>
   <si>
-    <t>helper plate (384 w- transparent)</t>
-  </si>
-  <si>
     <t>Assay I (384 w - white)</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Liha Tip Reservoirs</t>
   </si>
   <si>
-    <t>12 Col Overnight Strains</t>
-  </si>
-  <si>
     <t>A_subreservoir</t>
   </si>
   <si>
@@ -77,10 +71,16 @@
     <t>Tips</t>
   </si>
   <si>
-    <t xml:space="preserve">For IIb (and not for IIa) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Add second 12 Col overnight with prefilled columns</t>
+    <t xml:space="preserve"> Add second 384 transp, plate to cart 2, site 1 as next helper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For IIb (and not for IIa, IIc) </t>
+  </si>
+  <si>
+    <t>12 Col Overnight Strains (not for IIc)</t>
+  </si>
+  <si>
+    <t>helper plate (384 w- transparent). For Iic use pregrown helper</t>
   </si>
 </sst>
 </file>
@@ -161,12 +161,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -506,17 +511,17 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -528,7 +533,7 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
@@ -541,8 +546,8 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
+      <c r="A3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -554,8 +559,8 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
+      <c r="A4" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -567,8 +572,8 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
+      <c r="A5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -580,8 +585,8 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
+      <c r="A6" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -593,8 +598,8 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
+      <c r="A7" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -606,8 +611,8 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -619,8 +624,8 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -632,8 +637,8 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+      <c r="A10" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -645,8 +650,8 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
+      <c r="A11" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -658,8 +663,8 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
+      <c r="A12" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -671,8 +676,8 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
+      <c r="A13" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -684,13 +689,13 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
+      <c r="A14" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>14</v>
+      <c r="A15" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>

</xml_diff>